<commit_message>
Made minor changes to code files, created data file utilisation_ratio_state_wise_2010_2019.xlsx'
</commit_message>
<xml_diff>
--- a/Data/rice_wheat_expenditure.xlsx
+++ b/Data/rice_wheat_expenditure.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -21,36 +21,6 @@
   </si>
   <si>
     <t xml:space="preserve">wheat expenditure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2030</t>
   </si>
 </sst>
 </file>
@@ -394,113 +364,113 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" t="n">
+        <v>2021</v>
       </c>
       <c r="B2" t="n">
-        <v>73336.01748</v>
+        <v>73336.02</v>
       </c>
       <c r="C2" t="n">
-        <v>56765.45875</v>
+        <v>54750.39</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" t="n">
+        <v>2022</v>
       </c>
       <c r="B3" t="n">
-        <v>73966.1686</v>
+        <v>73966.17</v>
       </c>
       <c r="C3" t="n">
-        <v>57277.528</v>
+        <v>55238.76</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4" t="n">
+        <v>2023</v>
       </c>
       <c r="B4" t="n">
-        <v>74596.26368</v>
+        <v>74596.26</v>
       </c>
       <c r="C4" t="n">
-        <v>57789.655</v>
+        <v>55727.17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" t="n">
+        <v>2024</v>
       </c>
       <c r="B5" t="n">
-        <v>75226.3214</v>
+        <v>75226.32</v>
       </c>
       <c r="C5" t="n">
-        <v>58301.72425</v>
+        <v>56215.43</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" t="n">
+        <v>2025</v>
       </c>
       <c r="B6" t="n">
-        <v>75856.32308</v>
+        <v>75856.32</v>
       </c>
       <c r="C6" t="n">
-        <v>58813.601</v>
+        <v>56703.76</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>8</v>
+      <c r="A7" t="n">
+        <v>2026</v>
       </c>
       <c r="B7" t="n">
-        <v>76486.54892</v>
+        <v>76486.55</v>
       </c>
       <c r="C7" t="n">
-        <v>59325.70875</v>
+        <v>57192.15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>9</v>
+      <c r="A8" t="n">
+        <v>2027</v>
       </c>
       <c r="B8" t="n">
-        <v>77014.89404</v>
+        <v>77014.89</v>
       </c>
       <c r="C8" t="n">
-        <v>59755.0415</v>
+        <v>57601.68</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="A9" t="n">
+        <v>2028</v>
       </c>
       <c r="B9" t="n">
-        <v>77543.27652</v>
+        <v>77543.28</v>
       </c>
       <c r="C9" t="n">
-        <v>60184.48975</v>
+        <v>58011.2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>11</v>
+      <c r="A10" t="n">
+        <v>2029</v>
       </c>
       <c r="B10" t="n">
-        <v>78071.95788</v>
+        <v>78071.96</v>
       </c>
       <c r="C10" t="n">
-        <v>60614.11125</v>
+        <v>58420.9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" t="n">
+        <v>2030</v>
       </c>
       <c r="B11" t="n">
-        <v>78600.26564</v>
+        <v>78600.27</v>
       </c>
       <c r="C11" t="n">
-        <v>61043.46325</v>
+        <v>58830.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>